<commit_message>
actualizacion script, fallan prompts
</commit_message>
<xml_diff>
--- a/script_master_data/ficherosExcelOrigen/DED-EVsCaching_Adopcion IA_v1a.xlsx
+++ b/script_master_data/ficherosExcelOrigen/DED-EVsCaching_Adopcion IA_v1a.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85868A41-C1B2-4081-A32C-EB5C37120A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09010C34-DD48-420E-994A-E5D0054D3D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdopcionIA" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Estado" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AdopcionIA!$A$5:$AR$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AdopcionIA!$B$5:$AR$5</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="202">
   <si>
     <t>GISS-DED - Adopción IA: &lt;ProyectoEVs y Caching&gt;</t>
   </si>
@@ -689,7 +689,10 @@
       * A veces se meten demasiados caracteres y falla.</t>
   </si>
   <si>
-    <t>prompts</t>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>Documuentar</t>
   </si>
   <si>
     <t>Comprender Codigo Fuente</t>
@@ -748,7 +751,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -833,7 +835,6 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -853,7 +854,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -19472,16 +19472,16 @@
   <dimension ref="B2:AS106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AJ6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AQ6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AS6" sqref="AS6"/>
+      <selection pane="bottomRight" activeCell="AS4" sqref="AS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.26953125" style="1" customWidth="1"/>
     <col min="5" max="5" width="73.453125" style="1" customWidth="1"/>
@@ -19555,7 +19555,7 @@
       <c r="AN4" s="5"/>
       <c r="AO4" s="6"/>
     </row>
-    <row r="5" spans="2:45" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:45" ht="39" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -19685,11 +19685,11 @@
       <c r="AR5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AS5" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="121" t="s">
         <v>22</v>
       </c>
@@ -19785,11 +19785,11 @@
         <f>IF(OR(H6="S",M6="S",R6="S",W6="S",AB6="S",AG6="S",AL6="S"),"S","N")</f>
         <v>S</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AS6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:45" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:45" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="125" t="s">
         <v>22</v>
       </c>
@@ -19885,11 +19885,11 @@
         <f t="shared" ref="AR7:AR65" si="1">IF(OR(H7="S",M7="S",R7="S",W7="S",AB7="S",AG7="S",AL7="S"),"S","N")</f>
         <v>N</v>
       </c>
-      <c r="AS7" t="s">
-        <v>3</v>
+      <c r="AS7" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="8" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="125" t="s">
         <v>22</v>
       </c>
@@ -19971,11 +19971,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="AS8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="125" t="s">
         <v>22</v>
       </c>
@@ -20057,11 +20057,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
-      <c r="AS9" t="s">
-        <v>199</v>
+      <c r="AS9" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="10" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="125" t="s">
         <v>22</v>
       </c>
@@ -20159,11 +20159,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
-      <c r="AS10" t="s">
-        <v>200</v>
+      <c r="AS10" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="11" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="125" t="s">
         <v>22</v>
       </c>
@@ -20253,11 +20253,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AS11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="125" t="s">
         <v>22</v>
       </c>
@@ -20337,7 +20337,7 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AS12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -22667,7 +22667,9 @@
       <c r="E40" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="110"/>
+      <c r="F40" s="110" t="s">
+        <v>119</v>
+      </c>
       <c r="G40" s="116" t="s">
         <v>29</v>
       </c>
@@ -23121,7 +23123,9 @@
       <c r="E46" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="110"/>
+      <c r="F46" s="110" t="s">
+        <v>119</v>
+      </c>
       <c r="G46" s="116" t="s">
         <v>29</v>
       </c>
@@ -23190,7 +23194,9 @@
       <c r="E47" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="F47" s="110"/>
+      <c r="F47" s="110" t="s">
+        <v>32</v>
+      </c>
       <c r="G47" s="116" t="s">
         <v>29</v>
       </c>
@@ -26158,7 +26164,6 @@
       <c r="AR106" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:AR106" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="R28:S28 R12:S21 AG7:AH13 W7:X106 AB6:AC106 AL6:AM106 R34:S35 AG28:AH41 H6:I106 M8:N105 AG43:AH105">
     <cfRule type="expression" dxfId="108" priority="178">
       <formula>AND(G6="S",H6="")</formula>
@@ -30500,6 +30505,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c3e1b4bb-9124-477c-aa49-683b9a26b58f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E080B9D539EE5249B0F7896E1534F47F" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1a88378f58b9ad7590fd740332c19a90">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c298b4c-1b69-4120-abb9-a44ffc4bda23" xmlns:ns3="c3e1b4bb-9124-477c-aa49-683b9a26b58f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="910b3ddf48a2c6cdf16d80fb4d738ee7" ns2:_="" ns3:_="">
     <xsd:import namespace="8c298b4c-1b69-4120-abb9-a44ffc4bda23"/>
@@ -30700,30 +30728,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c3e1b4bb-9124-477c-aa49-683b9a26b58f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890994BF-65F0-45C5-A04B-1A065C31A5EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2E4D65A-0514-4AD4-B252-FA4173BA5D89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30740,22 +30763,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890994BF-65F0-45C5-A04B-1A065C31A5EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>